<commit_message>
Latest version Updated tests to comply to test script. Some minor changes in the tests to be documented.
</commit_message>
<xml_diff>
--- a/Support/RangeOperations.xlsx
+++ b/Support/RangeOperations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arjo\Projects\VS2019\Framework\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CDA7889-8367-4BD9-B718-201CFF3C17B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FE16A5-AE53-40FD-8B86-617AE72E4886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D19CF91-C312-4280-A670-70B431DF176A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4D19CF91-C312-4280-A670-70B431DF176A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>.</t>
   </si>
@@ -85,9 +85,6 @@
     <t>RangeMatch</t>
   </si>
   <si>
-    <t>Before</t>
-  </si>
-  <si>
     <t>EndsIn</t>
   </si>
   <si>
@@ -97,12 +94,6 @@
     <t>PartOf</t>
   </si>
   <si>
-    <t>After</t>
-  </si>
-  <si>
-    <t>Overlaps</t>
-  </si>
-  <si>
     <t>StartsIn</t>
   </si>
   <si>
@@ -167,6 +158,21 @@
   </si>
   <si>
     <t>Range(14,14)</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Tail</t>
+  </si>
+  <si>
+    <t>OutsideAfter</t>
+  </si>
+  <si>
+    <t>OutsideBefore</t>
+  </si>
+  <si>
+    <t>Overlap</t>
   </si>
 </sst>
 </file>
@@ -608,7 +614,7 @@
   <dimension ref="A2:AB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,10 +707,10 @@
         <v>15</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -778,13 +784,13 @@
         <v>-1</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="AA4" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -822,13 +828,13 @@
         <v>-1</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -866,13 +872,13 @@
         <v>-1</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -910,13 +916,13 @@
         <v>0</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -954,13 +960,13 @@
         <v>1</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -998,13 +1004,13 @@
         <v>1</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1042,13 +1048,13 @@
         <v>1</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1086,13 +1092,13 @@
         <v>1</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1130,18 +1136,18 @@
         <v>-1</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1172,18 +1178,18 @@
         <v>-1</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1214,18 +1220,18 @@
         <v>0</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1256,18 +1262,18 @@
         <v>0</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1298,18 +1304,18 @@
         <v>0</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="AA17" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB17" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1340,13 +1346,13 @@
         <v>1</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="AA18" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>